<commit_message>
Added PER material and type
</commit_message>
<xml_diff>
--- a/PipesCalculator/Resources/DATA.xlsx
+++ b/PipesCalculator/Resources/DATA.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Equipement" sheetId="1" r:id="rId1"/>
     <sheet name="Tube Cuivre" sheetId="2" r:id="rId2"/>
     <sheet name="Tube Acier" sheetId="3" r:id="rId3"/>
+    <sheet name="Tube PER" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -397,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -818,7 +820,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,4 +993,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B1">
+        <v>12</v>
+      </c>
+      <c r="C1">
+        <f>(A1*A1*PI())/4</f>
+        <v>75.429639612690949</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <f>(A2*A2*PI())/4</f>
+        <v>132.73228961416876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>16.2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f>(A3*A3*PI())/4</f>
+        <v>206.11989400202631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <f>(A4*A4*PI())/4</f>
+        <v>326.85129967948205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>26.2</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <f>(A5*A5*PI())/4</f>
+        <v>539.12871528254436</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>